<commit_message>
added product link of qoh
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaid7\Desktop\new_khwaahish\New folder\kh-admin-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC75EAF-F9D3-4530-AAD7-6D55AADC4EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CFE768-9ABF-46B7-8F39-B091C3AAE929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,12 +325,6 @@
     <t>https://abuzaid55-rittz-uploads-images-bucket.s3.ap-south-1.amazonaws.com/uploads/1741348205029_622458_NOOR_Banner_Header.jpg</t>
   </si>
   <si>
-    <t>https://abuzaid55-rittz-uploads-images-bucket.s3.ap-south-1.amazonaws.com/uploads/1741370589145_145949_bridal%20edit.jpg</t>
-  </si>
-  <si>
-    <t>14K</t>
-  </si>
-  <si>
     <t>Classic</t>
   </si>
   <si>
@@ -362,6 +356,12 @@
   </si>
   <si>
     <t>https://abuzaid55-rittz-uploads-images-bucket.s3.ap-south-1.amazonaws.com/uploads/1741543780112_387294_1.webp</t>
+  </si>
+  <si>
+    <t>https://abuzaid55-rittz-uploads-images-bucket.s3.ap-south-1.amazonaws.com/uploads/1741606977380_339523_GLER1002_RG0001.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18K </t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1618,8 @@
   <dimension ref="A1:BL154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K13" sqref="K13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2373,8 +2373,8 @@
       <c r="G6" s="12">
         <v>0</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>100</v>
+      <c r="H6" s="31" t="s">
+        <v>111</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -2382,7 +2382,7 @@
         <v>7</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>87</v>
@@ -2462,41 +2462,41 @@
       <c r="BJ6" s="9"/>
       <c r="BK6" s="9"/>
       <c r="BL6" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:64" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="G7" s="12">
         <v>10</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>87</v>
@@ -2517,14 +2517,14 @@
         <v>4</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U7" s="9">
         <v>11250</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AA7" s="9" t="s">
         <v>30</v>
@@ -10965,8 +10965,9 @@
     <hyperlink ref="H2" r:id="rId1" xr:uid="{82EA10D3-14EF-4673-9286-170AEAF93EAE}"/>
     <hyperlink ref="H5" r:id="rId2" xr:uid="{CAC98851-63DE-4897-BCAE-EE1BBB00E44E}"/>
     <hyperlink ref="H7" r:id="rId3" xr:uid="{A94415C7-D574-40D9-AC1F-1EA6B322D86D}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{CEF0FA6E-2592-4AB8-97C0-22C0D538D8B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>